<commit_message>
all functions moved to helper_functions.py
</commit_message>
<xml_diff>
--- a/Reports/Result_summary.xlsx
+++ b/Reports/Result_summary.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD264403-5355-4B07-9C07-F1686B439734}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D99EECA-8534-459A-A262-07EE9C973567}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="OneVsRest" sheetId="1" r:id="rId1"/>
-    <sheet name="Multi-Class Transformation" sheetId="4" r:id="rId2"/>
+    <sheet name="BinaryRelevance" sheetId="1" r:id="rId1"/>
+    <sheet name="LabelPowerset" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1722,7 @@
   <dimension ref="B2:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>